<commit_message>
Corrected Close CRM VBscript and added variable for BAU ST password
</commit_message>
<xml_diff>
--- a/Documents/Calendar/Calendar.xlsx
+++ b/Documents/Calendar/Calendar.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="PSPIE" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="30">
   <si>
     <t>TestCase</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>Adams</t>
-  </si>
-  <si>
-    <t>123123a</t>
   </si>
 </sst>
 </file>
@@ -500,7 +497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
@@ -609,7 +606,7 @@
         <v>24</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>21</v>
@@ -1044,7 +1041,7 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:J3"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1559,7 +1556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changed BAU user. Added generic credit risk page handling for all possible scenarios. Increased wait for DTV NPC load.
</commit_message>
<xml_diff>
--- a/Documents/Calendar/Calendar.xlsx
+++ b/Documents/Calendar/Calendar.xlsx
@@ -92,9 +92,6 @@
     <t>Please Specify</t>
   </si>
   <si>
-    <t>xx9381</t>
-  </si>
-  <si>
     <t>BAU ST</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>Adams</t>
+  </si>
+  <si>
+    <t>xx0770</t>
   </si>
 </sst>
 </file>
@@ -569,13 +569,13 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>17</v>
@@ -603,10 +603,10 @@
         <v>20</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>21</v>
@@ -620,13 +620,13 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>17</v>
@@ -654,10 +654,10 @@
         <v>20</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" s="5"/>
@@ -1041,7 +1041,7 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="M2" sqref="M2:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,13 +1104,13 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>17</v>
@@ -1138,10 +1138,10 @@
         <v>20</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>21</v>
@@ -1155,13 +1155,13 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>17</v>
@@ -1189,10 +1189,10 @@
         <v>20</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" s="5"/>
@@ -1215,7 +1215,7 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:J3"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,13 +1275,13 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>17</v>
@@ -1309,10 +1309,10 @@
         <v>20</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>21</v>
@@ -1326,13 +1326,13 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>17</v>
@@ -1360,10 +1360,10 @@
         <v>20</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" s="5"/>
@@ -1386,7 +1386,7 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:J3"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,13 +1446,13 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>17</v>
@@ -1480,10 +1480,10 @@
         <v>20</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>21</v>
@@ -1497,13 +1497,13 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>17</v>
@@ -1531,10 +1531,10 @@
         <v>20</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" s="5"/>
@@ -1557,10 +1557,13 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="17" max="17" width="20.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1617,13 +1620,13 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>17</v>
@@ -1651,10 +1654,10 @@
         <v>20</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>21</v>
@@ -1668,13 +1671,13 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>17</v>
@@ -1702,10 +1705,10 @@
         <v>20</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" s="5"/>

</xml_diff>

<commit_message>
Changed BAU user for UPIE to xx9381. xx0770 is SO for UPIe
</commit_message>
<xml_diff>
--- a/Documents/Calendar/Calendar.xlsx
+++ b/Documents/Calendar/Calendar.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="PSPIE" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="31">
   <si>
     <t>TestCase</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>xx0770</t>
+  </si>
+  <si>
+    <t>xx9381</t>
   </si>
 </sst>
 </file>
@@ -497,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,7 +1044,7 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:N2"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,7 +1218,7 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1556,7 +1559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
@@ -1654,10 +1657,10 @@
         <v>20</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>21</v>

</xml_diff>